<commit_message>
reviewed and updated by Cursor till payment
</commit_message>
<xml_diff>
--- a/气象/For_Python_站点信息和记录.xlsx
+++ b/气象/For_Python_站点信息和记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\文档\GIT SYNC\default\气象\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394321E0-3FB5-4AC8-90A9-5BECE6547370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56142EE-A18B-4ED6-AA58-16A1AC663DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2889" uniqueCount="783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2890" uniqueCount="784">
   <si>
     <t>id</t>
   </si>
@@ -2374,6 +2374,10 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Y</t>
@@ -3216,16 +3220,12 @@
       <c r="N2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="32">
-        <v>-29.2</v>
-      </c>
-      <c r="P2" s="32">
-        <v>-16.7</v>
-      </c>
-      <c r="Q2" s="32">
-        <v>-22.46</v>
-      </c>
-      <c r="R2" s="23"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="23" t="s">
+        <v>783</v>
+      </c>
       <c r="S2" s="37" t="s">
         <v>38</v>
       </c>
@@ -3496,15 +3496,9 @@
       <c r="N6" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="O6" s="32">
-        <v>-30</v>
-      </c>
-      <c r="P6" s="32">
-        <v>-11.4</v>
-      </c>
-      <c r="Q6" s="32">
-        <v>-23.09</v>
-      </c>
+      <c r="O6" s="32"/>
+      <c r="P6" s="32"/>
+      <c r="Q6" s="32"/>
       <c r="R6" s="23"/>
       <c r="S6" s="37" t="s">
         <v>38</v>
@@ -3648,15 +3642,9 @@
         <v>62</v>
       </c>
       <c r="N8" s="2"/>
-      <c r="O8" s="32">
-        <v>-30</v>
-      </c>
-      <c r="P8" s="32">
-        <v>-21</v>
-      </c>
-      <c r="Q8" s="32">
-        <v>-25.51</v>
-      </c>
+      <c r="O8" s="32"/>
+      <c r="P8" s="32"/>
+      <c r="Q8" s="32"/>
       <c r="R8" s="23" t="s">
         <v>38</v>
       </c>
@@ -3727,15 +3715,9 @@
         <v>66</v>
       </c>
       <c r="N9" s="2"/>
-      <c r="O9" s="32">
-        <v>-28.2</v>
-      </c>
-      <c r="P9" s="32">
-        <v>-17.2</v>
-      </c>
-      <c r="Q9" s="32">
-        <v>-23.76</v>
-      </c>
+      <c r="O9" s="32"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="32"/>
       <c r="R9" s="23" t="s">
         <v>38</v>
       </c>
@@ -3808,15 +3790,9 @@
         <v>68</v>
       </c>
       <c r="N10" s="3"/>
-      <c r="O10" s="32">
-        <v>-24.2</v>
-      </c>
-      <c r="P10" s="32">
-        <v>-16.8</v>
-      </c>
-      <c r="Q10" s="32">
-        <v>-20.75</v>
-      </c>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="32"/>
       <c r="R10" s="23" t="s">
         <v>38</v>
       </c>
@@ -3889,15 +3865,9 @@
       <c r="N11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="O11" s="32">
-        <v>-25.2</v>
-      </c>
-      <c r="P11" s="32">
-        <v>-12.4</v>
-      </c>
-      <c r="Q11" s="32">
-        <v>-16.18</v>
-      </c>
+      <c r="O11" s="32"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="32"/>
       <c r="R11" s="23" t="s">
         <v>38</v>
       </c>
@@ -3970,15 +3940,9 @@
         <v>73</v>
       </c>
       <c r="N12" s="2"/>
-      <c r="O12" s="32">
-        <v>-25</v>
-      </c>
-      <c r="P12" s="32">
-        <v>-14.6</v>
-      </c>
-      <c r="Q12" s="32">
-        <v>-20.54</v>
-      </c>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="32"/>
       <c r="R12" s="23" t="s">
         <v>38</v>
       </c>
@@ -4053,15 +4017,9 @@
       <c r="N13" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="O13" s="32">
-        <v>-29</v>
-      </c>
-      <c r="P13" s="32">
-        <v>-13.2</v>
-      </c>
-      <c r="Q13" s="32">
-        <v>-22.64</v>
-      </c>
+      <c r="O13" s="32"/>
+      <c r="P13" s="32"/>
+      <c r="Q13" s="32"/>
       <c r="R13" s="23" t="s">
         <v>38</v>
       </c>
@@ -4134,15 +4092,9 @@
         <v>77</v>
       </c>
       <c r="N14" s="2"/>
-      <c r="O14" s="32">
-        <v>-23.1</v>
-      </c>
-      <c r="P14" s="32">
-        <v>-14.4</v>
-      </c>
-      <c r="Q14" s="32">
-        <v>-18.96</v>
-      </c>
+      <c r="O14" s="32"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="32"/>
       <c r="R14" s="23" t="s">
         <v>38</v>
       </c>
@@ -4412,15 +4364,9 @@
         <v>86</v>
       </c>
       <c r="N18" s="2"/>
-      <c r="O18" s="32">
-        <v>-32.1</v>
-      </c>
-      <c r="P18" s="32">
-        <v>-21.4</v>
-      </c>
-      <c r="Q18" s="32">
-        <v>-28.1</v>
-      </c>
+      <c r="O18" s="32"/>
+      <c r="P18" s="32"/>
+      <c r="Q18" s="32"/>
       <c r="R18" s="23"/>
       <c r="S18" s="37"/>
       <c r="T18" s="2" t="s">
@@ -8113,15 +8059,9 @@
         <v>178</v>
       </c>
       <c r="N75" s="2"/>
-      <c r="O75" s="32">
-        <v>-24.4</v>
-      </c>
-      <c r="P75" s="32">
-        <v>-14.4</v>
-      </c>
-      <c r="Q75" s="32">
-        <v>-16.34</v>
-      </c>
+      <c r="O75" s="32"/>
+      <c r="P75" s="32"/>
+      <c r="Q75" s="32"/>
       <c r="R75" s="23" t="s">
         <v>38</v>
       </c>
@@ -8194,15 +8134,9 @@
         <v>184</v>
       </c>
       <c r="N76" s="2"/>
-      <c r="O76" s="32">
-        <v>-37.4</v>
-      </c>
-      <c r="P76" s="32">
-        <v>-24.8</v>
-      </c>
-      <c r="Q76" s="32">
-        <v>-29.33</v>
-      </c>
+      <c r="O76" s="32"/>
+      <c r="P76" s="32"/>
+      <c r="Q76" s="32"/>
       <c r="R76" s="23" t="s">
         <v>38</v>
       </c>
@@ -8277,15 +8211,9 @@
       <c r="N77" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="O77" s="32">
-        <v>-38.4</v>
-      </c>
-      <c r="P77" s="32">
-        <v>-21.5</v>
-      </c>
-      <c r="Q77" s="32">
-        <v>-30.14</v>
-      </c>
+      <c r="O77" s="32"/>
+      <c r="P77" s="32"/>
+      <c r="Q77" s="32"/>
       <c r="R77" s="23" t="s">
         <v>38</v>
       </c>
@@ -8358,15 +8286,9 @@
         <v>191</v>
       </c>
       <c r="N78" s="2"/>
-      <c r="O78" s="32">
-        <v>-34.299999999999997</v>
-      </c>
-      <c r="P78" s="32">
-        <v>-23.9</v>
-      </c>
-      <c r="Q78" s="32">
-        <v>-28.73</v>
-      </c>
+      <c r="O78" s="32"/>
+      <c r="P78" s="32"/>
+      <c r="Q78" s="32"/>
       <c r="R78" s="23" t="s">
         <v>38</v>
       </c>
@@ -8439,15 +8361,9 @@
       <c r="N79" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="O79" s="32">
-        <v>-35.1</v>
-      </c>
-      <c r="P79" s="32">
-        <v>-19.100000000000001</v>
-      </c>
-      <c r="Q79" s="32">
-        <v>-26.84</v>
-      </c>
+      <c r="O79" s="32"/>
+      <c r="P79" s="32"/>
+      <c r="Q79" s="32"/>
       <c r="R79" s="23" t="s">
         <v>38</v>
       </c>
@@ -8518,15 +8434,9 @@
         <v>197</v>
       </c>
       <c r="N80" s="2"/>
-      <c r="O80" s="32">
-        <v>-27.3</v>
-      </c>
-      <c r="P80" s="32">
-        <v>-23.5</v>
-      </c>
-      <c r="Q80" s="32">
-        <v>-25.88</v>
-      </c>
+      <c r="O80" s="32"/>
+      <c r="P80" s="32"/>
+      <c r="Q80" s="32"/>
       <c r="R80" s="23" t="s">
         <v>38</v>
       </c>
@@ -8601,15 +8511,9 @@
       <c r="N81" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="O81" s="32">
-        <v>-35.700000000000003</v>
-      </c>
-      <c r="P81" s="32">
-        <v>-25.5</v>
-      </c>
-      <c r="Q81" s="32">
-        <v>-31.86</v>
-      </c>
+      <c r="O81" s="32"/>
+      <c r="P81" s="32"/>
+      <c r="Q81" s="32"/>
       <c r="R81" s="23" t="s">
         <v>38</v>
       </c>
@@ -8686,15 +8590,9 @@
       <c r="N82" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="O82" s="32">
-        <v>-31</v>
-      </c>
-      <c r="P82" s="32">
-        <v>-17.5</v>
-      </c>
-      <c r="Q82" s="32">
-        <v>-21.64</v>
-      </c>
+      <c r="O82" s="32"/>
+      <c r="P82" s="32"/>
+      <c r="Q82" s="32"/>
       <c r="R82" s="23" t="s">
         <v>38</v>
       </c>
@@ -8767,15 +8665,9 @@
         <v>208</v>
       </c>
       <c r="N83" s="2"/>
-      <c r="O83" s="32">
-        <v>-26.9</v>
-      </c>
-      <c r="P83" s="32">
-        <v>-12.7</v>
-      </c>
-      <c r="Q83" s="32">
-        <v>-17.86</v>
-      </c>
+      <c r="O83" s="32"/>
+      <c r="P83" s="32"/>
+      <c r="Q83" s="32"/>
       <c r="R83" s="23" t="s">
         <v>38</v>
       </c>
@@ -8848,15 +8740,9 @@
       <c r="N84" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="O84" s="32">
-        <v>-30.7</v>
-      </c>
-      <c r="P84" s="32">
-        <v>-21.5</v>
-      </c>
-      <c r="Q84" s="32">
-        <v>-25.45</v>
-      </c>
+      <c r="O84" s="32"/>
+      <c r="P84" s="32"/>
+      <c r="Q84" s="32"/>
       <c r="R84" s="23" t="s">
         <v>38</v>
       </c>
@@ -8931,15 +8817,9 @@
       <c r="N85" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="O85" s="32">
-        <v>-20.399999999999999</v>
-      </c>
-      <c r="P85" s="32">
-        <v>-14.7</v>
-      </c>
-      <c r="Q85" s="32">
-        <v>-16.91</v>
-      </c>
+      <c r="O85" s="32"/>
+      <c r="P85" s="32"/>
+      <c r="Q85" s="32"/>
       <c r="R85" s="23" t="s">
         <v>38</v>
       </c>
@@ -9010,15 +8890,9 @@
         <v>221</v>
       </c>
       <c r="N86" s="2"/>
-      <c r="O86" s="32">
-        <v>-19.100000000000001</v>
-      </c>
-      <c r="P86" s="32">
-        <v>-13.9</v>
-      </c>
-      <c r="Q86" s="32">
-        <v>-16.64</v>
-      </c>
+      <c r="O86" s="32"/>
+      <c r="P86" s="32"/>
+      <c r="Q86" s="32"/>
       <c r="R86" s="23" t="s">
         <v>38</v>
       </c>
@@ -9097,15 +8971,9 @@
       <c r="N87" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="O87" s="32">
-        <v>-22.7</v>
-      </c>
-      <c r="P87" s="32">
-        <v>-16.8</v>
-      </c>
-      <c r="Q87" s="32">
-        <v>-20.61</v>
-      </c>
+      <c r="O87" s="32"/>
+      <c r="P87" s="32"/>
+      <c r="Q87" s="32"/>
       <c r="R87" s="23" t="s">
         <v>38</v>
       </c>
@@ -9176,15 +9044,9 @@
         <v>226</v>
       </c>
       <c r="N88" s="2"/>
-      <c r="O88" s="32">
-        <v>-19.399999999999999</v>
-      </c>
-      <c r="P88" s="32">
-        <v>-13.3</v>
-      </c>
-      <c r="Q88" s="32">
-        <v>-16.850000000000001</v>
-      </c>
+      <c r="O88" s="32"/>
+      <c r="P88" s="32"/>
+      <c r="Q88" s="32"/>
       <c r="R88" s="23" t="s">
         <v>38</v>
       </c>
@@ -9328,15 +9190,9 @@
       <c r="N90" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="O90" s="32">
-        <v>-22.8</v>
-      </c>
-      <c r="P90" s="32">
-        <v>-14</v>
-      </c>
-      <c r="Q90" s="32">
-        <v>-17.440000000000001</v>
-      </c>
+      <c r="O90" s="32"/>
+      <c r="P90" s="32"/>
+      <c r="Q90" s="32"/>
       <c r="R90" s="23" t="s">
         <v>38</v>
       </c>
@@ -9405,15 +9261,9 @@
         <v>239</v>
       </c>
       <c r="N91" s="2"/>
-      <c r="O91" s="32">
-        <v>-25.1</v>
-      </c>
-      <c r="P91" s="32">
-        <v>-18</v>
-      </c>
-      <c r="Q91" s="32">
-        <v>-20.62</v>
-      </c>
+      <c r="O91" s="32"/>
+      <c r="P91" s="32"/>
+      <c r="Q91" s="32"/>
       <c r="R91" s="23" t="s">
         <v>38</v>
       </c>
@@ -9482,15 +9332,9 @@
         <v>242</v>
       </c>
       <c r="N92" s="2"/>
-      <c r="O92" s="32">
-        <v>-10.8</v>
-      </c>
-      <c r="P92" s="32">
-        <v>-6.7</v>
-      </c>
-      <c r="Q92" s="32">
-        <v>-7.8</v>
-      </c>
+      <c r="O92" s="32"/>
+      <c r="P92" s="32"/>
+      <c r="Q92" s="32"/>
       <c r="R92" s="23" t="s">
         <v>38</v>
       </c>
@@ -9561,15 +9405,9 @@
         <v>247</v>
       </c>
       <c r="N93" s="2"/>
-      <c r="O93" s="32">
-        <v>-5.7</v>
-      </c>
-      <c r="P93" s="32">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="Q93" s="32">
-        <v>-0.37</v>
-      </c>
+      <c r="O93" s="32"/>
+      <c r="P93" s="32"/>
+      <c r="Q93" s="32"/>
       <c r="R93" s="23" t="s">
         <v>38</v>
       </c>
@@ -9645,10 +9483,10 @@
         <v>234</v>
       </c>
       <c r="O94" s="32">
-        <v>-15</v>
+        <v>-25.5</v>
       </c>
       <c r="P94" s="32">
-        <v>1.8</v>
+        <v>-6</v>
       </c>
       <c r="Q94" s="32"/>
       <c r="R94" s="23" t="s">
@@ -9725,15 +9563,9 @@
         <v>259</v>
       </c>
       <c r="N95" s="2"/>
-      <c r="O95" s="32">
-        <v>-13.4</v>
-      </c>
-      <c r="P95" s="32">
-        <v>-0.2</v>
-      </c>
-      <c r="Q95" s="32">
-        <v>-5.1100000000000003</v>
-      </c>
+      <c r="O95" s="32"/>
+      <c r="P95" s="32"/>
+      <c r="Q95" s="32"/>
       <c r="R95" s="23" t="s">
         <v>38</v>
       </c>
@@ -9812,12 +9644,8 @@
       <c r="N96" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="O96" s="32">
-        <v>-11.9</v>
-      </c>
-      <c r="P96" s="32">
-        <v>-0.4</v>
-      </c>
+      <c r="O96" s="32"/>
+      <c r="P96" s="32"/>
       <c r="Q96" s="32"/>
       <c r="R96" s="23" t="s">
         <v>38</v>
@@ -9893,15 +9721,9 @@
         <v>270</v>
       </c>
       <c r="N97" s="2"/>
-      <c r="O97" s="32">
-        <v>-15.7</v>
-      </c>
-      <c r="P97" s="32">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="Q97" s="32">
-        <v>-5.91</v>
-      </c>
+      <c r="O97" s="32"/>
+      <c r="P97" s="32"/>
+      <c r="Q97" s="32"/>
       <c r="R97" s="23" t="s">
         <v>38</v>
       </c>
@@ -9975,10 +9797,10 @@
       </c>
       <c r="N98" s="2"/>
       <c r="O98" s="32">
-        <v>-20</v>
+        <v>-26.2</v>
       </c>
       <c r="P98" s="32">
-        <v>-13.5</v>
+        <v>-13.7</v>
       </c>
       <c r="Q98" s="32"/>
       <c r="R98" s="23" t="s">
@@ -10055,15 +9877,9 @@
         <v>280</v>
       </c>
       <c r="N99" s="2"/>
-      <c r="O99" s="32">
-        <v>-29.2</v>
-      </c>
-      <c r="P99" s="32">
-        <v>-18.100000000000001</v>
-      </c>
-      <c r="Q99" s="32">
-        <v>-22.97</v>
-      </c>
+      <c r="O99" s="32"/>
+      <c r="P99" s="32"/>
+      <c r="Q99" s="32"/>
       <c r="R99" s="23" t="s">
         <v>38</v>
       </c>
@@ -10134,8 +9950,12 @@
         <v>284</v>
       </c>
       <c r="N100" s="2"/>
-      <c r="O100" s="32"/>
-      <c r="P100" s="32"/>
+      <c r="O100" s="32">
+        <v>-38.4</v>
+      </c>
+      <c r="P100" s="32">
+        <v>-21.6</v>
+      </c>
       <c r="Q100" s="32"/>
       <c r="R100" s="23" t="s">
         <v>38</v>
@@ -10208,10 +10028,10 @@
       </c>
       <c r="N101" s="2"/>
       <c r="O101" s="32">
-        <v>-35.799999999999997</v>
+        <v>-38.9</v>
       </c>
       <c r="P101" s="32">
-        <v>-23</v>
+        <v>-23.1</v>
       </c>
       <c r="Q101" s="32"/>
       <c r="R101" s="23" t="s">
@@ -10290,15 +10110,9 @@
         <v>291</v>
       </c>
       <c r="N102" s="2"/>
-      <c r="O102" s="32">
-        <v>-35.5</v>
-      </c>
-      <c r="P102" s="32">
-        <v>-23.6</v>
-      </c>
-      <c r="Q102" s="32">
-        <v>-30.16</v>
-      </c>
+      <c r="O102" s="32"/>
+      <c r="P102" s="32"/>
+      <c r="Q102" s="32"/>
       <c r="R102" s="23" t="s">
         <v>38</v>
       </c>
@@ -10371,12 +10185,8 @@
         <v>294</v>
       </c>
       <c r="N103" s="2"/>
-      <c r="O103" s="32">
-        <v>-34.4</v>
-      </c>
-      <c r="P103" s="32">
-        <v>-24.6</v>
-      </c>
+      <c r="O103" s="32"/>
+      <c r="P103" s="32"/>
       <c r="Q103" s="32"/>
       <c r="R103" s="23" t="s">
         <v>38</v>
@@ -10451,10 +10261,10 @@
       </c>
       <c r="N104" s="2"/>
       <c r="O104" s="32">
-        <v>-33</v>
+        <v>-39.4</v>
       </c>
       <c r="P104" s="32">
-        <v>-20.9</v>
+        <v>-22.9</v>
       </c>
       <c r="Q104" s="32"/>
       <c r="R104" s="23" t="s">
@@ -10535,15 +10345,9 @@
       <c r="N105" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="O105" s="32">
-        <v>-34.700000000000003</v>
-      </c>
-      <c r="P105" s="32">
-        <v>-20.3</v>
-      </c>
-      <c r="Q105" s="32">
-        <v>-28.85</v>
-      </c>
+      <c r="O105" s="32"/>
+      <c r="P105" s="32"/>
+      <c r="Q105" s="32"/>
       <c r="R105" s="23" t="s">
         <v>38</v>
       </c>
@@ -10621,10 +10425,10 @@
         <v>37</v>
       </c>
       <c r="O106" s="32">
-        <v>-32.9</v>
+        <v>-35.6</v>
       </c>
       <c r="P106" s="32">
-        <v>-23.2</v>
+        <v>-24.7</v>
       </c>
       <c r="Q106" s="32"/>
       <c r="R106" s="23" t="s">
@@ -10774,15 +10578,9 @@
         <v>308</v>
       </c>
       <c r="N108" s="2"/>
-      <c r="O108" s="32">
-        <v>-29.3</v>
-      </c>
-      <c r="P108" s="32">
-        <v>-18.5</v>
-      </c>
-      <c r="Q108" s="32">
-        <v>-24.29</v>
-      </c>
+      <c r="O108" s="32"/>
+      <c r="P108" s="32"/>
+      <c r="Q108" s="32"/>
       <c r="R108" s="23" t="s">
         <v>38</v>
       </c>
@@ -11001,15 +10799,9 @@
         <v>315</v>
       </c>
       <c r="N111" s="2"/>
-      <c r="O111" s="32">
-        <v>-25.9</v>
-      </c>
-      <c r="P111" s="32">
-        <v>-13.9</v>
-      </c>
-      <c r="Q111" s="32">
-        <v>-19.690000000000001</v>
-      </c>
+      <c r="O111" s="32"/>
+      <c r="P111" s="32"/>
+      <c r="Q111" s="32"/>
       <c r="R111" s="23" t="s">
         <v>38</v>
       </c>
@@ -11081,10 +10873,10 @@
       </c>
       <c r="N112" s="2"/>
       <c r="O112" s="32">
-        <v>-18.5</v>
+        <v>-20</v>
       </c>
       <c r="P112" s="32">
-        <v>-2.4</v>
+        <v>-8.8000000000000007</v>
       </c>
       <c r="Q112" s="32"/>
       <c r="R112" s="23" t="s">
@@ -11156,10 +10948,10 @@
       </c>
       <c r="N113" s="2"/>
       <c r="O113" s="32">
-        <v>-15.6</v>
+        <v>-18.3</v>
       </c>
       <c r="P113" s="32">
-        <v>2.2999999999999998</v>
+        <v>-2.1</v>
       </c>
       <c r="Q113" s="32"/>
       <c r="R113" s="23" t="s">
@@ -11235,10 +11027,10 @@
         <v>83</v>
       </c>
       <c r="O114" s="32">
-        <v>-15.6</v>
+        <v>-22.9</v>
       </c>
       <c r="P114" s="32">
-        <v>3.1</v>
+        <v>-0.8</v>
       </c>
       <c r="Q114" s="32"/>
       <c r="R114" s="23" t="s">
@@ -11317,12 +11109,8 @@
       <c r="N115" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="O115" s="32">
-        <v>-18.8</v>
-      </c>
-      <c r="P115" s="32">
-        <v>-1.9</v>
-      </c>
+      <c r="O115" s="32"/>
+      <c r="P115" s="32"/>
       <c r="Q115" s="32"/>
       <c r="R115" s="23" t="s">
         <v>38</v>
@@ -11398,15 +11186,9 @@
         <v>335</v>
       </c>
       <c r="N116" s="2"/>
-      <c r="O116" s="32">
-        <v>-19.100000000000001</v>
-      </c>
-      <c r="P116" s="32">
-        <v>-1.2</v>
-      </c>
-      <c r="Q116" s="32">
-        <v>-10.61</v>
-      </c>
+      <c r="O116" s="32"/>
+      <c r="P116" s="32"/>
+      <c r="Q116" s="32"/>
       <c r="R116" s="23" t="s">
         <v>38</v>
       </c>
@@ -11478,10 +11260,10 @@
       </c>
       <c r="N117" s="2"/>
       <c r="O117" s="32">
-        <v>-19.3</v>
+        <v>-20.3</v>
       </c>
       <c r="P117" s="32">
-        <v>-5.0999999999999996</v>
+        <v>-5.5</v>
       </c>
       <c r="Q117" s="32"/>
       <c r="R117" s="23" t="s">
@@ -11557,10 +11339,10 @@
         <v>234</v>
       </c>
       <c r="O118" s="32">
-        <v>-31.1</v>
+        <v>-29.6</v>
       </c>
       <c r="P118" s="32">
-        <v>-17.100000000000001</v>
+        <v>-15.5</v>
       </c>
       <c r="Q118" s="32"/>
       <c r="R118" s="23" t="s">
@@ -11637,15 +11419,9 @@
         <v>348</v>
       </c>
       <c r="N119" s="2"/>
-      <c r="O119" s="32">
-        <v>-21.5</v>
-      </c>
-      <c r="P119" s="32">
-        <v>-8.8000000000000007</v>
-      </c>
-      <c r="Q119" s="32">
-        <v>-16.850000000000001</v>
-      </c>
+      <c r="O119" s="32"/>
+      <c r="P119" s="32"/>
+      <c r="Q119" s="32"/>
       <c r="R119" s="23" t="s">
         <v>38</v>
       </c>
@@ -11722,15 +11498,9 @@
         <v>353</v>
       </c>
       <c r="N120" s="2"/>
-      <c r="O120" s="32">
-        <v>-7.5</v>
-      </c>
-      <c r="P120" s="32">
-        <v>-0.2</v>
-      </c>
-      <c r="Q120" s="32">
-        <v>-4.3499999999999996</v>
-      </c>
+      <c r="O120" s="32"/>
+      <c r="P120" s="32"/>
+      <c r="Q120" s="32"/>
       <c r="R120" s="23" t="s">
         <v>38</v>
       </c>
@@ -11803,15 +11573,9 @@
         <v>358</v>
       </c>
       <c r="N121" s="2"/>
-      <c r="O121" s="32">
-        <v>-9.6999999999999993</v>
-      </c>
-      <c r="P121" s="32">
-        <v>-6</v>
-      </c>
-      <c r="Q121" s="32">
-        <v>-8.1300000000000008</v>
-      </c>
+      <c r="O121" s="32"/>
+      <c r="P121" s="32"/>
+      <c r="Q121" s="32"/>
       <c r="R121" s="23" t="s">
         <v>38</v>
       </c>
@@ -11888,12 +11652,8 @@
         <v>363</v>
       </c>
       <c r="N122" s="2"/>
-      <c r="O122" s="32">
-        <v>-25.7</v>
-      </c>
-      <c r="P122" s="32">
-        <v>-14.2</v>
-      </c>
+      <c r="O122" s="32"/>
+      <c r="P122" s="32"/>
       <c r="Q122" s="32"/>
       <c r="R122" s="23" t="s">
         <v>38</v>
@@ -12044,15 +11804,9 @@
         <v>371</v>
       </c>
       <c r="N124" s="2"/>
-      <c r="O124" s="32">
-        <v>-12</v>
-      </c>
-      <c r="P124" s="32">
-        <v>-0.7</v>
-      </c>
-      <c r="Q124" s="32">
-        <v>-6.02</v>
-      </c>
+      <c r="O124" s="32"/>
+      <c r="P124" s="32"/>
+      <c r="Q124" s="32"/>
       <c r="R124" s="23" t="s">
         <v>38</v>
       </c>
@@ -12129,15 +11883,9 @@
         <v>376</v>
       </c>
       <c r="N125" s="2"/>
-      <c r="O125" s="32">
-        <v>-1.9</v>
-      </c>
-      <c r="P125" s="32">
-        <v>6.7</v>
-      </c>
-      <c r="Q125" s="32">
-        <v>2.75</v>
-      </c>
+      <c r="O125" s="32"/>
+      <c r="P125" s="32"/>
+      <c r="Q125" s="32"/>
       <c r="R125" s="23" t="s">
         <v>38</v>
       </c>
@@ -12203,10 +11951,10 @@
       </c>
       <c r="N126" s="2"/>
       <c r="O126" s="32">
-        <v>1</v>
+        <v>-2.2999999999999998</v>
       </c>
       <c r="P126" s="32">
-        <v>8.5</v>
+        <v>7.6</v>
       </c>
       <c r="Q126" s="32"/>
       <c r="R126" s="23" t="s">
@@ -12279,15 +12027,9 @@
         <v>384</v>
       </c>
       <c r="N127" s="2"/>
-      <c r="O127" s="32">
-        <v>-5.7</v>
-      </c>
-      <c r="P127" s="32">
-        <v>2.9</v>
-      </c>
-      <c r="Q127" s="32">
-        <v>-0.89</v>
-      </c>
+      <c r="O127" s="32"/>
+      <c r="P127" s="32"/>
+      <c r="Q127" s="32"/>
       <c r="R127" s="23" t="s">
         <v>38</v>
       </c>
@@ -12362,12 +12104,8 @@
         <v>390</v>
       </c>
       <c r="N128" s="2"/>
-      <c r="O128" s="32">
-        <v>-0.5</v>
-      </c>
-      <c r="P128" s="32">
-        <v>11</v>
-      </c>
+      <c r="O128" s="32"/>
+      <c r="P128" s="32"/>
       <c r="Q128" s="32"/>
       <c r="R128" s="23" t="s">
         <v>38</v>
@@ -12439,15 +12177,9 @@
         <v>394</v>
       </c>
       <c r="N129" s="2"/>
-      <c r="O129" s="32">
-        <v>-2.2000000000000002</v>
-      </c>
-      <c r="P129" s="32">
-        <v>5.4</v>
-      </c>
-      <c r="Q129" s="32">
-        <v>2.21</v>
-      </c>
+      <c r="O129" s="32"/>
+      <c r="P129" s="32"/>
+      <c r="Q129" s="32"/>
       <c r="R129" s="23" t="s">
         <v>38</v>
       </c>
@@ -12522,15 +12254,9 @@
         <v>400</v>
       </c>
       <c r="N130" s="2"/>
-      <c r="O130" s="32">
-        <v>-7.4</v>
-      </c>
-      <c r="P130" s="32">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="Q130" s="32">
-        <v>-3.39</v>
-      </c>
+      <c r="O130" s="32"/>
+      <c r="P130" s="32"/>
+      <c r="Q130" s="32"/>
       <c r="R130" s="23" t="s">
         <v>38</v>
       </c>
@@ -12605,15 +12331,9 @@
         <v>405</v>
       </c>
       <c r="N131" s="2"/>
-      <c r="O131" s="32">
-        <v>-0.2</v>
-      </c>
-      <c r="P131" s="32">
-        <v>5.8</v>
-      </c>
-      <c r="Q131" s="32">
-        <v>2.77</v>
-      </c>
+      <c r="O131" s="32"/>
+      <c r="P131" s="32"/>
+      <c r="Q131" s="32"/>
       <c r="R131" s="23" t="s">
         <v>38</v>
       </c>
@@ -12686,15 +12406,9 @@
         <v>411</v>
       </c>
       <c r="N132" s="2"/>
-      <c r="O132" s="32">
-        <v>2.9</v>
-      </c>
-      <c r="P132" s="32">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="Q132" s="32">
-        <v>6.51</v>
-      </c>
+      <c r="O132" s="32"/>
+      <c r="P132" s="32"/>
+      <c r="Q132" s="32"/>
       <c r="R132" s="23" t="s">
         <v>38</v>
       </c>
@@ -12767,15 +12481,9 @@
         <v>417</v>
       </c>
       <c r="N133" s="2"/>
-      <c r="O133" s="32">
-        <v>3.3</v>
-      </c>
-      <c r="P133" s="32">
-        <v>10</v>
-      </c>
-      <c r="Q133" s="32">
-        <v>6.44</v>
-      </c>
+      <c r="O133" s="32"/>
+      <c r="P133" s="32"/>
+      <c r="Q133" s="32"/>
       <c r="R133" s="23" t="s">
         <v>38</v>
       </c>
@@ -12850,15 +12558,9 @@
         <v>424</v>
       </c>
       <c r="N134" s="2"/>
-      <c r="O134" s="32">
-        <v>5.5</v>
-      </c>
-      <c r="P134" s="32">
-        <v>8.4</v>
-      </c>
-      <c r="Q134" s="32">
-        <v>6.55</v>
-      </c>
+      <c r="O134" s="32"/>
+      <c r="P134" s="32"/>
+      <c r="Q134" s="32"/>
       <c r="R134" s="23" t="s">
         <v>38</v>
       </c>
@@ -12929,15 +12631,9 @@
         <v>429</v>
       </c>
       <c r="N135" s="2"/>
-      <c r="O135" s="32">
-        <v>7.3</v>
-      </c>
-      <c r="P135" s="32">
-        <v>11.8</v>
-      </c>
-      <c r="Q135" s="32">
-        <v>8.9</v>
-      </c>
+      <c r="O135" s="32"/>
+      <c r="P135" s="32"/>
+      <c r="Q135" s="32"/>
       <c r="R135" s="23" t="s">
         <v>38</v>
       </c>
@@ -13010,15 +12706,9 @@
         <v>435</v>
       </c>
       <c r="N136" s="2"/>
-      <c r="O136" s="32">
-        <v>10.4</v>
-      </c>
-      <c r="P136" s="32">
-        <v>14.2</v>
-      </c>
-      <c r="Q136" s="32">
-        <v>11.81</v>
-      </c>
+      <c r="O136" s="32"/>
+      <c r="P136" s="32"/>
+      <c r="Q136" s="32"/>
       <c r="R136" s="23" t="s">
         <v>38</v>
       </c>
@@ -13091,15 +12781,9 @@
         <v>441</v>
       </c>
       <c r="N137" s="2"/>
-      <c r="O137" s="32">
-        <v>6.7</v>
-      </c>
-      <c r="P137" s="32">
-        <v>10.6</v>
-      </c>
-      <c r="Q137" s="32">
-        <v>7.75</v>
-      </c>
+      <c r="O137" s="32"/>
+      <c r="P137" s="32"/>
+      <c r="Q137" s="32"/>
       <c r="R137" s="23" t="s">
         <v>38</v>
       </c>
@@ -13172,12 +12856,8 @@
         <v>447</v>
       </c>
       <c r="N138" s="2"/>
-      <c r="O138" s="32">
-        <v>5.7</v>
-      </c>
-      <c r="P138" s="32">
-        <v>8.9</v>
-      </c>
+      <c r="O138" s="32"/>
+      <c r="P138" s="32"/>
       <c r="Q138" s="32"/>
       <c r="R138" s="23" t="s">
         <v>38</v>
@@ -13251,15 +12931,9 @@
         <v>453</v>
       </c>
       <c r="N139" s="2"/>
-      <c r="O139" s="32">
-        <v>7</v>
-      </c>
-      <c r="P139" s="32">
-        <v>10.4</v>
-      </c>
-      <c r="Q139" s="32">
-        <v>8.65</v>
-      </c>
+      <c r="O139" s="32"/>
+      <c r="P139" s="32"/>
+      <c r="Q139" s="32"/>
       <c r="R139" s="23" t="s">
         <v>38</v>
       </c>
@@ -13332,15 +13006,9 @@
         <v>458</v>
       </c>
       <c r="N140" s="2"/>
-      <c r="O140" s="32">
-        <v>7</v>
-      </c>
-      <c r="P140" s="32">
-        <v>16.399999999999999</v>
-      </c>
-      <c r="Q140" s="32">
-        <v>10.38</v>
-      </c>
+      <c r="O140" s="32"/>
+      <c r="P140" s="32"/>
+      <c r="Q140" s="32"/>
       <c r="R140" s="23" t="s">
         <v>38</v>
       </c>
@@ -13413,15 +13081,9 @@
         <v>464</v>
       </c>
       <c r="N141" s="2"/>
-      <c r="O141" s="32">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="P141" s="32">
-        <v>19.399999999999999</v>
-      </c>
-      <c r="Q141" s="32">
-        <v>13.31</v>
-      </c>
+      <c r="O141" s="32"/>
+      <c r="P141" s="32"/>
+      <c r="Q141" s="32"/>
       <c r="R141" s="23" t="s">
         <v>38</v>
       </c>
@@ -13492,15 +13154,9 @@
         <v>469</v>
       </c>
       <c r="N142" s="2"/>
-      <c r="O142" s="32">
-        <v>13.5</v>
-      </c>
-      <c r="P142" s="32">
-        <v>22.9</v>
-      </c>
-      <c r="Q142" s="32">
-        <v>17.05</v>
-      </c>
+      <c r="O142" s="32"/>
+      <c r="P142" s="32"/>
+      <c r="Q142" s="32"/>
       <c r="R142" s="23" t="s">
         <v>38</v>
       </c>
@@ -13573,15 +13229,9 @@
         <v>475</v>
       </c>
       <c r="N143" s="2"/>
-      <c r="O143" s="32">
-        <v>15.5</v>
-      </c>
-      <c r="P143" s="32">
-        <v>25.3</v>
-      </c>
-      <c r="Q143" s="32">
-        <v>19.440000000000001</v>
-      </c>
+      <c r="O143" s="32"/>
+      <c r="P143" s="32"/>
+      <c r="Q143" s="32"/>
       <c r="R143" s="23" t="s">
         <v>38</v>
       </c>
@@ -13654,15 +13304,9 @@
         <v>481</v>
       </c>
       <c r="N144" s="2"/>
-      <c r="O144" s="32">
-        <v>21.1</v>
-      </c>
-      <c r="P144" s="32">
-        <v>26.3</v>
-      </c>
-      <c r="Q144" s="32">
-        <v>22.93</v>
-      </c>
+      <c r="O144" s="32"/>
+      <c r="P144" s="32"/>
+      <c r="Q144" s="32"/>
       <c r="R144" s="23" t="s">
         <v>38</v>
       </c>
@@ -13733,15 +13377,9 @@
         <v>486</v>
       </c>
       <c r="N145" s="2"/>
-      <c r="O145" s="32">
-        <v>19.3</v>
-      </c>
-      <c r="P145" s="32">
-        <v>24</v>
-      </c>
-      <c r="Q145" s="32">
-        <v>20.91</v>
-      </c>
+      <c r="O145" s="32"/>
+      <c r="P145" s="32"/>
+      <c r="Q145" s="32"/>
       <c r="R145" s="23" t="s">
         <v>38</v>
       </c>
@@ -13810,15 +13448,9 @@
         <v>490</v>
       </c>
       <c r="N146" s="2"/>
-      <c r="O146" s="32">
-        <v>21.8</v>
-      </c>
-      <c r="P146" s="32">
-        <v>26.2</v>
-      </c>
-      <c r="Q146" s="32">
-        <v>24.21</v>
-      </c>
+      <c r="O146" s="32"/>
+      <c r="P146" s="32"/>
+      <c r="Q146" s="32"/>
       <c r="R146" s="23" t="s">
         <v>38</v>
       </c>
@@ -13887,15 +13519,9 @@
         <v>493</v>
       </c>
       <c r="N147" s="2"/>
-      <c r="O147" s="32">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="P147" s="32">
-        <v>22.6</v>
-      </c>
-      <c r="Q147" s="32">
-        <v>19.64</v>
-      </c>
+      <c r="O147" s="32"/>
+      <c r="P147" s="32"/>
+      <c r="Q147" s="32"/>
       <c r="R147" s="23" t="s">
         <v>38</v>
       </c>
@@ -13968,12 +13594,8 @@
         <v>499</v>
       </c>
       <c r="N148" s="2"/>
-      <c r="O148" s="32">
-        <v>13.1</v>
-      </c>
-      <c r="P148" s="32">
-        <v>20.6</v>
-      </c>
+      <c r="O148" s="32"/>
+      <c r="P148" s="32"/>
       <c r="Q148" s="32"/>
       <c r="R148" s="23" t="s">
         <v>38</v>
@@ -14045,15 +13667,9 @@
         <v>504</v>
       </c>
       <c r="N149" s="2"/>
-      <c r="O149" s="32">
-        <v>5.3</v>
-      </c>
-      <c r="P149" s="32">
-        <v>12.4</v>
-      </c>
-      <c r="Q149" s="32">
-        <v>9.18</v>
-      </c>
+      <c r="O149" s="32"/>
+      <c r="P149" s="32"/>
+      <c r="Q149" s="32"/>
       <c r="R149" s="23" t="s">
         <v>38</v>
       </c>
@@ -14126,15 +13742,9 @@
         <v>509</v>
       </c>
       <c r="N150" s="2"/>
-      <c r="O150" s="32">
-        <v>6</v>
-      </c>
-      <c r="P150" s="32">
-        <v>13.9</v>
-      </c>
-      <c r="Q150" s="32">
-        <v>8</v>
-      </c>
+      <c r="O150" s="32"/>
+      <c r="P150" s="32"/>
+      <c r="Q150" s="32"/>
       <c r="R150" s="23" t="s">
         <v>38</v>
       </c>
@@ -14207,15 +13817,9 @@
         <v>515</v>
       </c>
       <c r="N151" s="2"/>
-      <c r="O151" s="32">
-        <v>10.1</v>
-      </c>
-      <c r="P151" s="32">
-        <v>13.1</v>
-      </c>
-      <c r="Q151" s="32">
-        <v>11.16</v>
-      </c>
+      <c r="O151" s="32"/>
+      <c r="P151" s="32"/>
+      <c r="Q151" s="32"/>
       <c r="R151" s="23" t="s">
         <v>38</v>
       </c>
@@ -14355,15 +13959,9 @@
         <v>524</v>
       </c>
       <c r="N153" s="2"/>
-      <c r="O153" s="32">
-        <v>3.5</v>
-      </c>
-      <c r="P153" s="32">
-        <v>15</v>
-      </c>
-      <c r="Q153" s="32">
-        <v>9.8000000000000007</v>
-      </c>
+      <c r="O153" s="32"/>
+      <c r="P153" s="32"/>
+      <c r="Q153" s="32"/>
       <c r="R153" s="23" t="s">
         <v>38</v>
       </c>
@@ -14438,15 +14036,9 @@
         <v>530</v>
       </c>
       <c r="N154" s="2"/>
-      <c r="O154" s="32">
-        <v>-3.9</v>
-      </c>
-      <c r="P154" s="32">
-        <v>15.4</v>
-      </c>
-      <c r="Q154" s="32">
-        <v>2.58</v>
-      </c>
+      <c r="O154" s="32"/>
+      <c r="P154" s="32"/>
+      <c r="Q154" s="32"/>
       <c r="R154" s="23" t="s">
         <v>38</v>
       </c>
@@ -14585,10 +14177,10 @@
       </c>
       <c r="N156" s="2"/>
       <c r="O156" s="32">
-        <v>-13.3</v>
+        <v>-21</v>
       </c>
       <c r="P156" s="32">
-        <v>-0.5</v>
+        <v>-4</v>
       </c>
       <c r="Q156" s="32"/>
       <c r="R156" s="23" t="s">
@@ -14660,10 +14252,10 @@
       </c>
       <c r="N157" s="2"/>
       <c r="O157" s="32">
-        <v>10.3</v>
+        <v>8.4</v>
       </c>
       <c r="P157" s="32">
-        <v>16.899999999999999</v>
+        <v>11.8</v>
       </c>
       <c r="Q157" s="32"/>
       <c r="R157" s="23" t="s">
@@ -14940,10 +14532,10 @@
       </c>
       <c r="N161" s="2"/>
       <c r="O161" s="32">
-        <v>-2.8</v>
+        <v>-4.9000000000000004</v>
       </c>
       <c r="P161" s="32">
-        <v>5.0999999999999996</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="Q161" s="32"/>
       <c r="R161" s="23" t="s">
@@ -15238,10 +14830,10 @@
         <v>48</v>
       </c>
       <c r="O165" s="32">
-        <v>-38.200000000000003</v>
+        <v>-44.9</v>
       </c>
       <c r="P165" s="32">
-        <v>-23.6</v>
+        <v>-26.8</v>
       </c>
       <c r="Q165" s="32"/>
       <c r="R165" s="23" t="s">
@@ -15814,10 +15406,10 @@
       </c>
       <c r="N173" s="2"/>
       <c r="O173" s="32">
-        <v>-19</v>
+        <v>-24.7</v>
       </c>
       <c r="P173" s="32">
-        <v>-5.8</v>
+        <v>-10.3</v>
       </c>
       <c r="Q173" s="32"/>
       <c r="R173" s="23" t="s">
@@ -16032,12 +15624,8 @@
         <v>599</v>
       </c>
       <c r="N176" s="2"/>
-      <c r="O176" s="32">
-        <v>4.7</v>
-      </c>
-      <c r="P176" s="32">
-        <v>7.9</v>
-      </c>
+      <c r="O176" s="32"/>
+      <c r="P176" s="32"/>
       <c r="Q176" s="32"/>
       <c r="R176" s="23" t="s">
         <v>38</v>
@@ -16104,10 +15692,10 @@
       </c>
       <c r="N177" s="2"/>
       <c r="O177" s="32">
-        <v>-17.399999999999999</v>
+        <v>-20.6</v>
       </c>
       <c r="P177" s="32">
-        <v>-12.5</v>
+        <v>-15.3</v>
       </c>
       <c r="Q177" s="32"/>
       <c r="R177" s="23" t="s">
@@ -16724,15 +16312,9 @@
         <v>631</v>
       </c>
       <c r="N186" s="2"/>
-      <c r="O186" s="32">
-        <v>-54.6</v>
-      </c>
-      <c r="P186" s="32">
-        <v>-51.4</v>
-      </c>
-      <c r="Q186" s="32">
-        <v>-53.38</v>
-      </c>
+      <c r="O186" s="32"/>
+      <c r="P186" s="32"/>
+      <c r="Q186" s="32"/>
       <c r="R186" s="23" t="s">
         <v>38</v>
       </c>
@@ -16801,15 +16383,9 @@
         <v>634</v>
       </c>
       <c r="N187" s="2"/>
-      <c r="O187" s="32">
-        <v>-53.5</v>
-      </c>
-      <c r="P187" s="32">
-        <v>-48</v>
-      </c>
-      <c r="Q187" s="32">
-        <v>-52.36</v>
-      </c>
+      <c r="O187" s="32"/>
+      <c r="P187" s="32"/>
+      <c r="Q187" s="32"/>
       <c r="R187" s="23" t="s">
         <v>38</v>
       </c>
@@ -16876,15 +16452,9 @@
         <v>636</v>
       </c>
       <c r="N188" s="2"/>
-      <c r="O188" s="32">
-        <v>-51</v>
-      </c>
-      <c r="P188" s="32">
-        <v>-47.1</v>
-      </c>
-      <c r="Q188" s="32">
-        <v>-49.54</v>
-      </c>
+      <c r="O188" s="32"/>
+      <c r="P188" s="32"/>
+      <c r="Q188" s="32"/>
       <c r="R188" s="23" t="s">
         <v>38</v>
       </c>
@@ -16951,15 +16521,9 @@
         <v>637</v>
       </c>
       <c r="N189" s="2"/>
-      <c r="O189" s="32">
-        <v>-57</v>
-      </c>
-      <c r="P189" s="32">
-        <v>-52.4</v>
-      </c>
-      <c r="Q189" s="32">
-        <v>-54.85</v>
-      </c>
+      <c r="O189" s="32"/>
+      <c r="P189" s="32"/>
+      <c r="Q189" s="32"/>
       <c r="R189" s="23" t="s">
         <v>38</v>
       </c>
@@ -17026,15 +16590,9 @@
         <v>639</v>
       </c>
       <c r="N190" s="2"/>
-      <c r="O190" s="32">
-        <v>-53.8</v>
-      </c>
-      <c r="P190" s="32">
-        <v>-51.5</v>
-      </c>
-      <c r="Q190" s="32">
-        <v>-52.4</v>
-      </c>
+      <c r="O190" s="32"/>
+      <c r="P190" s="32"/>
+      <c r="Q190" s="32"/>
       <c r="R190" s="23" t="s">
         <v>38</v>
       </c>
@@ -17101,15 +16659,9 @@
         <v>642</v>
       </c>
       <c r="N191" s="2"/>
-      <c r="O191" s="32">
-        <v>-53.5</v>
-      </c>
-      <c r="P191" s="32">
-        <v>-49.6</v>
-      </c>
-      <c r="Q191" s="32">
-        <v>-51.85</v>
-      </c>
+      <c r="O191" s="32"/>
+      <c r="P191" s="32"/>
+      <c r="Q191" s="32"/>
       <c r="R191" s="23" t="s">
         <v>38</v>
       </c>
@@ -17174,15 +16726,9 @@
         <v>644</v>
       </c>
       <c r="N192" s="2"/>
-      <c r="O192" s="32">
-        <v>-50.4</v>
-      </c>
-      <c r="P192" s="32">
-        <v>-45.9</v>
-      </c>
-      <c r="Q192" s="32">
-        <v>-48.97</v>
-      </c>
+      <c r="O192" s="32"/>
+      <c r="P192" s="32"/>
+      <c r="Q192" s="32"/>
       <c r="R192" s="23" t="s">
         <v>38</v>
       </c>
@@ -17249,15 +16795,9 @@
         <v>647</v>
       </c>
       <c r="N193" s="2"/>
-      <c r="O193" s="32">
-        <v>-44.4</v>
-      </c>
-      <c r="P193" s="32">
-        <v>-42.4</v>
-      </c>
-      <c r="Q193" s="32">
-        <v>-43.5</v>
-      </c>
+      <c r="O193" s="32"/>
+      <c r="P193" s="32"/>
+      <c r="Q193" s="32"/>
       <c r="R193" s="23" t="s">
         <v>38</v>
       </c>
@@ -17326,12 +16866,8 @@
         <v>649</v>
       </c>
       <c r="N194" s="2"/>
-      <c r="O194" s="32">
-        <v>-55.6</v>
-      </c>
-      <c r="P194" s="32">
-        <v>-52.1</v>
-      </c>
+      <c r="O194" s="32"/>
+      <c r="P194" s="32"/>
       <c r="Q194" s="32"/>
       <c r="R194" s="23" t="s">
         <v>38</v>
@@ -17399,15 +16935,9 @@
         <v>652</v>
       </c>
       <c r="N195" s="2"/>
-      <c r="O195" s="32">
-        <v>-41.6</v>
-      </c>
-      <c r="P195" s="32">
-        <v>-33.4</v>
-      </c>
-      <c r="Q195" s="32">
-        <v>-36.53</v>
-      </c>
+      <c r="O195" s="32"/>
+      <c r="P195" s="32"/>
+      <c r="Q195" s="32"/>
       <c r="R195" s="23" t="s">
         <v>38</v>
       </c>
@@ -17476,15 +17006,9 @@
         <v>655</v>
       </c>
       <c r="N196" s="2"/>
-      <c r="O196" s="32">
-        <v>-44.7</v>
-      </c>
-      <c r="P196" s="32">
-        <v>-36</v>
-      </c>
-      <c r="Q196" s="32">
-        <v>-39.6</v>
-      </c>
+      <c r="O196" s="32"/>
+      <c r="P196" s="32"/>
+      <c r="Q196" s="32"/>
       <c r="R196" s="23" t="s">
         <v>38</v>
       </c>
@@ -17551,15 +17075,9 @@
         <v>660</v>
       </c>
       <c r="N197" s="24"/>
-      <c r="O197" s="32">
-        <v>-49.1</v>
-      </c>
-      <c r="P197" s="32">
-        <v>-46.7</v>
-      </c>
-      <c r="Q197" s="32">
-        <v>-48.61</v>
-      </c>
+      <c r="O197" s="32"/>
+      <c r="P197" s="32"/>
+      <c r="Q197" s="32"/>
       <c r="R197" s="23" t="s">
         <v>38</v>
       </c>
@@ -17691,8 +17209,12 @@
         <v>666</v>
       </c>
       <c r="N199" s="2"/>
-      <c r="O199" s="32"/>
-      <c r="P199" s="32"/>
+      <c r="O199" s="32">
+        <v>-40.299999999999997</v>
+      </c>
+      <c r="P199" s="32">
+        <v>-22.9</v>
+      </c>
       <c r="Q199" s="32"/>
       <c r="R199" s="23" t="s">
         <v>38</v>
@@ -17829,8 +17351,12 @@
         <v>669</v>
       </c>
       <c r="N201" s="2"/>
-      <c r="O201" s="32"/>
-      <c r="P201" s="32"/>
+      <c r="O201" s="32">
+        <v>-43</v>
+      </c>
+      <c r="P201" s="32">
+        <v>-22.8</v>
+      </c>
       <c r="Q201" s="32"/>
       <c r="R201" s="23" t="s">
         <v>38</v>
@@ -18584,12 +18110,8 @@
         <v>695</v>
       </c>
       <c r="N212" s="2"/>
-      <c r="O212" s="32">
-        <v>-37.1</v>
-      </c>
-      <c r="P212" s="32">
-        <v>-25.2</v>
-      </c>
+      <c r="O212" s="32"/>
+      <c r="P212" s="32"/>
       <c r="Q212" s="32"/>
       <c r="R212" s="23" t="s">
         <v>38</v>
@@ -18653,15 +18175,9 @@
         <v>698</v>
       </c>
       <c r="N213" s="2"/>
-      <c r="O213" s="32">
-        <v>-12.6</v>
-      </c>
-      <c r="P213" s="32">
-        <v>-1.3</v>
-      </c>
-      <c r="Q213" s="32">
-        <v>-4.99</v>
-      </c>
+      <c r="O213" s="32"/>
+      <c r="P213" s="32"/>
+      <c r="Q213" s="32"/>
       <c r="R213" s="23" t="s">
         <v>38</v>
       </c>
@@ -18732,15 +18248,9 @@
         <v>702</v>
       </c>
       <c r="N214" s="2"/>
-      <c r="O214" s="32">
-        <v>-22</v>
-      </c>
-      <c r="P214" s="32">
-        <v>-14.3</v>
-      </c>
-      <c r="Q214" s="32">
-        <v>-18.38</v>
-      </c>
+      <c r="O214" s="32"/>
+      <c r="P214" s="32"/>
+      <c r="Q214" s="32"/>
       <c r="R214" s="23" t="s">
         <v>38</v>
       </c>
@@ -18813,15 +18323,9 @@
         <v>705</v>
       </c>
       <c r="N215" s="2"/>
-      <c r="O215" s="32">
-        <v>-23.4</v>
-      </c>
-      <c r="P215" s="32">
-        <v>-13.7</v>
-      </c>
-      <c r="Q215" s="32">
-        <v>-19.75</v>
-      </c>
+      <c r="O215" s="32"/>
+      <c r="P215" s="32"/>
+      <c r="Q215" s="32"/>
       <c r="R215" s="23" t="s">
         <v>38</v>
       </c>
@@ -18894,15 +18398,9 @@
         <v>708</v>
       </c>
       <c r="N216" s="2"/>
-      <c r="O216" s="32">
-        <v>-26.4</v>
-      </c>
-      <c r="P216" s="32">
-        <v>-15.3</v>
-      </c>
-      <c r="Q216" s="32">
-        <v>-18.41</v>
-      </c>
+      <c r="O216" s="32"/>
+      <c r="P216" s="32"/>
+      <c r="Q216" s="32"/>
       <c r="R216" s="23" t="s">
         <v>38</v>
       </c>
@@ -18973,15 +18471,9 @@
         <v>711</v>
       </c>
       <c r="N217" s="2"/>
-      <c r="O217" s="32">
-        <v>-10.9</v>
-      </c>
-      <c r="P217" s="32">
-        <v>-8.1</v>
-      </c>
-      <c r="Q217" s="32">
-        <v>-9.19</v>
-      </c>
+      <c r="O217" s="32"/>
+      <c r="P217" s="32"/>
+      <c r="Q217" s="32"/>
       <c r="R217" s="23" t="s">
         <v>38</v>
       </c>
@@ -19052,15 +18544,9 @@
         <v>715</v>
       </c>
       <c r="N218" s="2"/>
-      <c r="O218" s="32">
-        <v>-19.600000000000001</v>
-      </c>
-      <c r="P218" s="32">
-        <v>-16.399999999999999</v>
-      </c>
-      <c r="Q218" s="32">
-        <v>-17.78</v>
-      </c>
+      <c r="O218" s="32"/>
+      <c r="P218" s="32"/>
+      <c r="Q218" s="32"/>
       <c r="R218" s="23" t="s">
         <v>38</v>
       </c>
@@ -19131,15 +18617,9 @@
         <v>718</v>
       </c>
       <c r="N219" s="2"/>
-      <c r="O219" s="32">
-        <v>-8.4</v>
-      </c>
-      <c r="P219" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="Q219" s="32">
-        <v>-3.46</v>
-      </c>
+      <c r="O219" s="32"/>
+      <c r="P219" s="32"/>
+      <c r="Q219" s="32"/>
       <c r="R219" s="23" t="s">
         <v>38</v>
       </c>
@@ -19204,8 +18684,12 @@
         <v>722</v>
       </c>
       <c r="N220" s="2"/>
-      <c r="O220" s="32"/>
-      <c r="P220" s="32"/>
+      <c r="O220" s="32">
+        <v>-44.1</v>
+      </c>
+      <c r="P220" s="32">
+        <v>-21.4</v>
+      </c>
       <c r="Q220" s="32"/>
       <c r="R220" s="23" t="s">
         <v>38</v>
@@ -19411,12 +18895,8 @@
         <v>729</v>
       </c>
       <c r="N223" s="2"/>
-      <c r="O223" s="32">
-        <v>-33.9</v>
-      </c>
-      <c r="P223" s="32">
-        <v>-26.3</v>
-      </c>
+      <c r="O223" s="32"/>
+      <c r="P223" s="32"/>
       <c r="Q223" s="32"/>
       <c r="R223" s="23" t="s">
         <v>38</v>
@@ -19484,8 +18964,12 @@
         <v>731</v>
       </c>
       <c r="N224" s="2"/>
-      <c r="O224" s="32"/>
-      <c r="P224" s="32"/>
+      <c r="O224" s="32">
+        <v>-43.3</v>
+      </c>
+      <c r="P224" s="32">
+        <v>-22.5</v>
+      </c>
       <c r="Q224" s="32"/>
       <c r="R224" s="23" t="s">
         <v>38</v>
@@ -19751,10 +19235,10 @@
       </c>
       <c r="N228" s="2"/>
       <c r="O228" s="32">
-        <v>-36.1</v>
+        <v>-40.9</v>
       </c>
       <c r="P228" s="32">
-        <v>-26.2</v>
+        <v>-27.7</v>
       </c>
       <c r="Q228" s="32"/>
       <c r="R228" s="23" t="s">
@@ -20025,10 +19509,10 @@
       </c>
       <c r="N232" s="2"/>
       <c r="O232" s="32">
-        <v>-38.5</v>
+        <v>-44.3</v>
       </c>
       <c r="P232" s="32">
-        <v>-24.9</v>
+        <v>-26.3</v>
       </c>
       <c r="Q232" s="32"/>
       <c r="R232" s="23" t="s">

</xml_diff>